<commit_message>
feat: add force light theme
</commit_message>
<xml_diff>
--- a/Cronograma/PLAN_SEQUENCIAMENTO.xlsx
+++ b/Cronograma/PLAN_SEQUENCIAMENTO.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="1300" documentId="8_{A7D517F8-C21C-42B1-847A-02B452B788FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5623F41-D6EE-4C4B-ACDD-18F31FE0C8DA}"/>
+  <xr:revisionPtr revIDLastSave="1308" documentId="8_{A7D517F8-C21C-42B1-847A-02B452B788FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9CB251F-7ACF-4D4B-9CDA-838DBAEDD234}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="17" r:id="rId1"/>
@@ -2952,9 +2952,9 @@
   </sheetPr>
   <dimension ref="A1:BY54"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BT20" sqref="BT20"/>
       <extLst>
         <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
           <xlsdti:showDataTypeIcons visible="0"/>
@@ -5004,9 +5004,7 @@
         <v>53</v>
       </c>
       <c r="C17" s="42"/>
-      <c r="E17" s="18">
-        <v>0</v>
-      </c>
+      <c r="E17" s="18"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="20">
@@ -6041,7 +6039,7 @@
       <c r="C22" s="42"/>
       <c r="D22" s="17"/>
       <c r="E22" s="18">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
@@ -6282,7 +6280,7 @@
       <c r="C23" s="42"/>
       <c r="D23" s="17"/>
       <c r="E23" s="18">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
@@ -6523,7 +6521,7 @@
       <c r="C24" s="42"/>
       <c r="D24" s="17"/>
       <c r="E24" s="18">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -7305,7 +7303,9 @@
         <v>71</v>
       </c>
       <c r="C28" s="42"/>
-      <c r="E28" s="18"/>
+      <c r="E28" s="18">
+        <v>1</v>
+      </c>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
       <c r="H28" s="20"/>
@@ -7371,7 +7371,9 @@
         <v>72</v>
       </c>
       <c r="C29" s="42"/>
-      <c r="E29" s="18"/>
+      <c r="E29" s="18">
+        <v>1</v>
+      </c>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
       <c r="H29" s="20"/>
@@ -7442,10 +7444,7 @@
       <c r="E30" s="18">
         <v>1</v>
       </c>
-      <c r="F30" s="11">
-        <f t="shared" ref="F30:F34" si="24">$F$4</f>
-        <v>45910</v>
-      </c>
+      <c r="F30" s="11"/>
       <c r="G30" s="19"/>
       <c r="H30" s="20"/>
       <c r="I30" s="17"/>
@@ -7683,10 +7682,7 @@
       <c r="E31" s="18">
         <v>1</v>
       </c>
-      <c r="F31" s="11">
-        <f t="shared" si="24"/>
-        <v>45910</v>
-      </c>
+      <c r="F31" s="11"/>
       <c r="G31" s="40"/>
     </row>
     <row r="32" spans="1:65" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7698,10 +7694,7 @@
       <c r="E32" s="18">
         <v>1</v>
       </c>
-      <c r="F32" s="11">
-        <f t="shared" si="24"/>
-        <v>45910</v>
-      </c>
+      <c r="F32" s="11"/>
       <c r="G32" s="40"/>
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7713,10 +7706,7 @@
       <c r="E33" s="18">
         <v>1</v>
       </c>
-      <c r="F33" s="11">
-        <f t="shared" si="24"/>
-        <v>45910</v>
-      </c>
+      <c r="F33" s="11"/>
       <c r="G33" s="19"/>
     </row>
     <row r="34" spans="2:7" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7726,10 +7716,7 @@
       <c r="C34" s="42"/>
       <c r="D34" s="42"/>
       <c r="E34" s="18"/>
-      <c r="F34" s="11">
-        <f t="shared" si="24"/>
-        <v>45910</v>
-      </c>
+      <c r="F34" s="11"/>
       <c r="G34" s="19"/>
     </row>
     <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -8029,8 +8016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{417B25A2-62B7-4D4C-82D1-AB533628D66B}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>